<commit_message>
new file:   README.md 	modified:   env/result.xlsx 	new file:   screenshots/bulk_search.png 	new file:   screenshots/dashboard.png 	new file:   screenshots/home.png 	new file:   screenshots/login.png 	new file:   screenshots/single_search.png
</commit_message>
<xml_diff>
--- a/env/result.xlsx
+++ b/env/result.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="11620" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="181029" fullCalcOnLoad="1"/>
@@ -424,18 +424,23 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A6" sqref="A6:A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="10.625" defaultRowHeight="15.75"/>
   <cols>
     <col width="12.125" bestFit="1" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Phone Number</t>
+        </is>
+      </c>
       <c r="B1" t="inlineStr">
         <is>
           <t>ID</t>
@@ -462,33 +467,30 @@
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>Phone Number</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
         <is>
           <t>city</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>9212433299</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>+919446933709</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Z8WgmB10VpRR4qgXX7w2bQ==</t>
+          <t>asmoggEczlaJI9aJKUw3qg==</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bhav Goyal</t>
+          <t>Cdr Manu Vidyarthi</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>0.32841069</t>
+          <t>0.3222276</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -498,37 +500,29 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+919212433299</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Delhi</t>
+          <t>Kerala</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>9212633299</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>+919447433709</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>MBdLyjF8xsOYq3T6QrNJeg==</t>
+          <t>uaef4zP1ky/K+u5/LAMhUw==</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bhav Goyal</t>
+          <t>Subani</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.9</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>https://storage.googleapis.com/tc-images-noneu/myview/1/57caf73f0abd306786b8e8c797913acb/1</t>
+          <t>0.3168635</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -538,32 +532,29 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>+919212633299</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Delhi</t>
+          <t>Kerala</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>9212100508</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>+918891911108</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>N6bRy3AImt/E6eHSLhjLcg==</t>
+          <t>xdVTVN9NhWSSadKauFRPMg==</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Rajneesh Goyal</t>
+          <t>Subani Vidyarthi</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.9</t>
+          <t>0.30928558</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -573,32 +564,29 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>+919212100508</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Delhi</t>
+          <t>Kerala</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>7982578104</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>+919854291183</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>LXm6OVf/SEd5xwke6QonPA==</t>
+          <t>toIIhLeJJ1wo5K1S6qA7Mw==</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Anju Maheshwari</t>
+          <t>Barnali Bhagabati</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>0.31463495</t>
+          <t>0.30918905</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -608,47 +596,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>+917982578104</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Delhi</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>8800889139</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>ACwvbX+YrOGOgCPkDdt+yA==</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Hardik</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>0.32487288</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>PUBLIC</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>+918800889139</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Delhi</t>
+          <t>Assam</t>
         </is>
       </c>
     </row>

</xml_diff>